<commit_message>
Finish variant 8 #22, 23 and 26
</commit_message>
<xml_diff>
--- a/ЕГЭ/Варианты/2024/Вариант 8/files/22.xlsx
+++ b/ЕГЭ/Варианты/2024/Вариант 8/files/22.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -58,7 +58,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -81,11 +81,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -99,9 +110,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -117,9 +137,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +177,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -229,7 +249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -403,20 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C13"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -428,7 +448,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -438,10 +458,15 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2</v>
+      </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -452,9 +477,18 @@
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
+      <c r="F3" s="5">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5</v>
+      </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -464,8 +498,44 @@
       <c r="C4" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>13</v>
+      </c>
+      <c r="Q4">
+        <v>14</v>
+      </c>
+      <c r="R4">
+        <v>15</v>
+      </c>
+      <c r="S4">
+        <v>16</v>
+      </c>
+      <c r="T4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -475,8 +545,29 @@
       <c r="C5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -486,8 +577,11 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -497,8 +591,26 @@
       <c r="C7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>11</v>
+      </c>
+      <c r="O7">
+        <v>12</v>
+      </c>
+      <c r="P7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -508,8 +620,26 @@
       <c r="C8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6">
+        <v>4</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -519,8 +649,26 @@
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="U9">
+        <v>18</v>
+      </c>
+      <c r="V9">
+        <v>19</v>
+      </c>
+      <c r="W9">
+        <v>20</v>
+      </c>
+      <c r="X9">
+        <v>21</v>
+      </c>
+      <c r="Y9">
+        <v>22</v>
+      </c>
+      <c r="Z9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -530,8 +678,20 @@
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -541,8 +701,41 @@
       <c r="C11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3</v>
+      </c>
+      <c r="G11" s="6">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6">
+        <v>5</v>
+      </c>
+      <c r="I11" s="6">
+        <v>6</v>
+      </c>
+      <c r="J11" s="6">
+        <v>7</v>
+      </c>
+      <c r="K11" s="6">
+        <v>8</v>
+      </c>
+      <c r="L11" s="6">
+        <v>9</v>
+      </c>
+      <c r="M11" s="6">
+        <v>10</v>
+      </c>
+      <c r="N11" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -552,8 +745,26 @@
       <c r="C12" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="AA12">
+        <v>24</v>
+      </c>
+      <c r="AB12">
+        <v>25</v>
+      </c>
+      <c r="AC12">
+        <v>26</v>
+      </c>
+      <c r="AD12">
+        <v>27</v>
+      </c>
+      <c r="AE12">
+        <v>28</v>
+      </c>
+      <c r="AF12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -563,13 +774,32 @@
       <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P13">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>14</v>
+      </c>
+      <c r="R13">
+        <v>15</v>
+      </c>
+      <c r="S13">
+        <v>16</v>
+      </c>
+      <c r="T13">
+        <v>17</v>
+      </c>
+      <c r="U13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>